<commit_message>
modified:   index.js 	modified:   salida.xlsx
</commit_message>
<xml_diff>
--- a/salida.xlsx
+++ b/salida.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bvr217\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F65EFA59-E243-4656-9424-091D6A4587F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD664CC0-A6CA-411B-A407-768151585067}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1065" yWindow="915" windowWidth="16200" windowHeight="11985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>asdsa</t>
   </si>
@@ -37,6 +37,12 @@
   </si>
   <si>
     <t>Brayan vargas Rojas</t>
+  </si>
+  <si>
+    <t>Mariana Conde</t>
+  </si>
+  <si>
+    <t>dsfasdfsadf</t>
   </si>
 </sst>
 </file>
@@ -354,10 +360,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -387,6 +393,17 @@
         <v>3166746160</v>
       </c>
     </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>3125048463</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>